<commit_message>
Integração Pandas x Excel
</commit_message>
<xml_diff>
--- a/BD.xlsx
+++ b/BD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HFBiBru\Meu Drive (haroldo.metzker@rio.rj.gov.br)\temp\ipea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HFBiBru\PycharmProjects\Projeto-SMTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{808DA3E1-16DF-4FA6-BFDC-9BE827CB948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AA50BF-2EB9-43E8-8BB8-5928774F41D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{562EA06A-641A-45B5-B845-CFBDBC377A56}"/>
   </bookViews>
@@ -37,16 +37,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
+    <t>ano</t>
+  </si>
+  <si>
     <t>km coberto</t>
   </si>
   <si>
     <t>pax pagantes</t>
   </si>
   <si>
-    <t>ano</t>
-  </si>
-  <si>
-    <t>mês</t>
+    <t>mes</t>
   </si>
 </sst>
 </file>
@@ -70,27 +70,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -102,7 +87,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -422,7 +407,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,17 +419,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>